<commit_message>
report backend 80%  was finished
</commit_message>
<xml_diff>
--- a/kds medical urls.xlsx
+++ b/kds medical urls.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lalith\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lalith\Desktop\Development\2020 Project Class BIT\Student Project - 2020\kdsMedical\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8CDA3941-97A6-4751-8B52-951A8ACE83B6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C60F3CF-2584-449F-972B-9AE4C2B3EE41}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3615" yWindow="720" windowWidth="15375" windowHeight="7995" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="51">
   <si>
     <t>Main Part</t>
   </si>
@@ -150,26 +150,50 @@
     <t>mainWindow</t>
   </si>
   <si>
-    <t>Receptionist</t>
-  </si>
-  <si>
-    <t>Doctor</t>
-  </si>
-  <si>
-    <t>Nurses</t>
+    <t>additional</t>
+  </si>
+  <si>
+    <t>card</t>
+  </si>
+  <si>
+    <t>cash</t>
+  </si>
+  <si>
+    <t>valid</t>
+  </si>
+  <si>
+    <t>ADMIN</t>
+  </si>
+  <si>
+    <t>CASHIER</t>
+  </si>
+  <si>
+    <t>MANAGER</t>
+  </si>
+  <si>
+    <t>ACCOUNTANT</t>
+  </si>
+  <si>
+    <t>HR_MANAGER</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10.5"/>
+      <color rgb="FF7EC3E6"/>
+      <name val="Inconsolata"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -192,8 +216,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -532,38 +559,47 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I85"/>
+  <dimension ref="A1:K91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="C43" sqref="C43"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="7" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="7.140625" customWidth="1"/>
-    <col min="2" max="2" width="27.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="9" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11">
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="G1" t="s">
-        <v>42</v>
-      </c>
-      <c r="H1" t="s">
-        <v>43</v>
-      </c>
-      <c r="I1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
       <c r="A2">
         <v>1</v>
       </c>
@@ -571,12 +607,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11">
       <c r="C3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11">
       <c r="C4" t="s">
         <v>4</v>
       </c>
@@ -584,7 +620,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11">
       <c r="C5" t="s">
         <v>6</v>
       </c>
@@ -592,7 +628,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11">
       <c r="C6" t="s">
         <v>7</v>
       </c>
@@ -600,12 +636,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11">
       <c r="C7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11">
       <c r="A9">
         <v>2</v>
       </c>
@@ -613,12 +649,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11">
       <c r="C10" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11">
       <c r="A12">
         <v>3</v>
       </c>
@@ -629,7 +665,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11">
       <c r="A14">
         <v>4</v>
       </c>
@@ -637,12 +673,12 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11">
       <c r="C15" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11">
       <c r="C16" t="s">
         <v>12</v>
       </c>
@@ -650,7 +686,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4">
       <c r="C17" t="s">
         <v>13</v>
       </c>
@@ -658,7 +694,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4">
       <c r="C18" t="s">
         <v>14</v>
       </c>
@@ -666,7 +702,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4">
       <c r="A20">
         <v>5</v>
       </c>
@@ -674,12 +710,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4">
       <c r="C21" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4">
       <c r="C22" t="s">
         <v>4</v>
       </c>
@@ -687,7 +723,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4">
       <c r="C23" t="s">
         <v>6</v>
       </c>
@@ -695,7 +731,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4">
       <c r="A25">
         <v>6</v>
       </c>
@@ -703,12 +739,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4">
       <c r="C26" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4">
       <c r="C27" t="s">
         <v>4</v>
       </c>
@@ -716,7 +752,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4">
       <c r="C28" t="s">
         <v>6</v>
       </c>
@@ -724,7 +760,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4">
       <c r="A30">
         <v>7</v>
       </c>
@@ -732,12 +768,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4">
       <c r="C31" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4">
       <c r="C32" t="s">
         <v>18</v>
       </c>
@@ -745,7 +781,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4">
       <c r="C33" t="s">
         <v>6</v>
       </c>
@@ -753,7 +789,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4">
       <c r="C34" t="s">
         <v>19</v>
       </c>
@@ -761,12 +797,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4">
       <c r="C35" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4">
       <c r="A37">
         <v>8</v>
       </c>
@@ -774,12 +810,12 @@
         <v>20</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4">
       <c r="C38" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4">
       <c r="C39" t="s">
         <v>6</v>
       </c>
@@ -787,7 +823,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4">
       <c r="C40" t="s">
         <v>21</v>
       </c>
@@ -795,7 +831,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4">
       <c r="C41" t="s">
         <v>19</v>
       </c>
@@ -803,17 +839,17 @@
         <v>5</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4">
       <c r="C42" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4">
       <c r="C43" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4">
       <c r="A45">
         <v>9</v>
       </c>
@@ -824,7 +860,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4">
       <c r="A47">
         <v>10</v>
       </c>
@@ -832,7 +868,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4">
       <c r="A49">
         <v>11</v>
       </c>
@@ -840,7 +876,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4">
       <c r="A51">
         <v>12</v>
       </c>
@@ -848,12 +884,12 @@
         <v>27</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4">
       <c r="C52" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4">
       <c r="C53" t="s">
         <v>6</v>
       </c>
@@ -861,7 +897,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4">
       <c r="C54" t="s">
         <v>19</v>
       </c>
@@ -869,27 +905,27 @@
         <v>5</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4">
       <c r="C55" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4">
       <c r="C56" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4">
       <c r="C57" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4">
       <c r="C58" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4">
       <c r="A60">
         <v>13</v>
       </c>
@@ -897,149 +933,180 @@
         <v>30</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4">
       <c r="C61" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63">
+    <row r="62" spans="1:4">
+      <c r="C62" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4">
+      <c r="C63" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4">
+      <c r="C64" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4">
+      <c r="C65" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4">
+      <c r="C66" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4">
+      <c r="C67" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4">
+      <c r="A69">
         <v>14</v>
       </c>
-      <c r="B63" t="s">
+      <c r="B69" t="s">
         <v>31</v>
       </c>
-      <c r="C63" t="s">
+      <c r="C69" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C64" t="s">
+    <row r="70" spans="1:4">
+      <c r="C70" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66">
+    <row r="72" spans="1:4">
+      <c r="A72">
         <v>15</v>
       </c>
-      <c r="B66" t="s">
+      <c r="B72" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C67" t="s">
+    <row r="73" spans="1:4">
+      <c r="C73" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C68" t="s">
+    <row r="74" spans="1:4">
+      <c r="C74" t="s">
         <v>6</v>
       </c>
-      <c r="D68" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C69" t="s">
+      <c r="D74" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4">
+      <c r="C75" t="s">
         <v>19</v>
       </c>
-      <c r="D69" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C70" t="s">
+      <c r="D75" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4">
+      <c r="C76" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C71" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73">
+    <row r="77" spans="1:4">
+      <c r="C77" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4">
+      <c r="A79">
         <v>16</v>
       </c>
-      <c r="B73" t="s">
+      <c r="B79" t="s">
         <v>35</v>
       </c>
-      <c r="C73" t="s">
+      <c r="C79" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C74" t="s">
+    <row r="80" spans="1:4">
+      <c r="C80" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C75" t="s">
+    <row r="81" spans="1:4">
+      <c r="C81" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C76" t="s">
+    <row r="82" spans="1:4">
+      <c r="C82" t="s">
         <v>38</v>
       </c>
-      <c r="D76" t="s">
+      <c r="D82" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C77" t="s">
+    <row r="83" spans="1:4">
+      <c r="C83" t="s">
         <v>38</v>
       </c>
-      <c r="D77" t="s">
+      <c r="D83" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C78" t="s">
+    <row r="84" spans="1:4">
+      <c r="C84" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80">
+    <row r="86" spans="1:4">
+      <c r="A86">
         <v>17</v>
       </c>
-      <c r="B80" t="s">
+      <c r="B86" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="81" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C81" t="s">
+    <row r="87" spans="1:4">
+      <c r="C87" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="82" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C82" t="s">
+    <row r="88" spans="1:4">
+      <c r="C88" t="s">
         <v>6</v>
       </c>
-      <c r="D82" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="83" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C83" t="s">
+      <c r="D88" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4">
+      <c r="C89" t="s">
         <v>19</v>
       </c>
-      <c r="D83" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="84" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C84" t="s">
+      <c r="D89" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4">
+      <c r="C90" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="85" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C85" t="s">
+    <row r="91" spans="1:4">
+      <c r="C91" t="s">
         <v>5</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1049,7 +1116,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1061,7 +1128,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
nav bar was updated
</commit_message>
<xml_diff>
--- a/kds medical urls.xlsx
+++ b/kds medical urls.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lalith\Desktop\Development\2020 Project Class BIT\Student Project - 2020\kdsMedical\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C60F3CF-2584-449F-972B-9AE4C2B3EE41}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11E467E4-1AC5-438A-B6C9-A2B0A53F8EB5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -561,8 +561,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="B60" sqref="B60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7" defaultRowHeight="15"/>

</xml_diff>